<commit_message>
feat (tuan 5): add
</commit_message>
<xml_diff>
--- a/tuan 3 add.xlsx
+++ b/tuan 3 add.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BABBC1-0F47-4D17-8B1F-E69C1D8F9246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1EE11-FD70-4FF2-B7F8-38995406478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
     <sheet name="2.MoTaSP" sheetId="2" r:id="rId2"/>
+    <sheet name="4.KeHoachXucTien" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>(5) Chi phí hoạt động</t>
   </si>
@@ -134,7 +132,49 @@
     <t>Thêm chức năng cho các hệ thống có sẵn</t>
   </si>
   <si>
-    <t>Thêm các chức năng hoặc sửa lại giao diện có sẵn theo yêu cầu của khách hàng</t>
+    <t>Thêm các chức năng hoặc sửa lại giao diện từ mã nguồn cũ theo yêu cầu của khách hàng</t>
+  </si>
+  <si>
+    <t>Tư vấn nâng cấp các hệ thống phần mềm cũ</t>
+  </si>
+  <si>
+    <t>Tư vấn giải pháp, giá cả nâng cấp cho các hệ thống cũ của khách hàng.</t>
+  </si>
+  <si>
+    <t>Chi phí</t>
+  </si>
+  <si>
+    <t>Thời gian thực hiện</t>
+  </si>
+  <si>
+    <t>Chăm sóc khách hàng</t>
+  </si>
+  <si>
+    <t>Với người tiêu dùng</t>
+  </si>
+  <si>
+    <t>Các trung gian phân phối</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Có thể vận chuyển 1 mặt hàng từ 1-2 ngày </t>
+  </si>
+  <si>
+    <t>Vận chuyển trong 1 ngày, thời gian sớm nhất</t>
+  </si>
+  <si>
+    <t>5.000.000 – 10.000.000</t>
+  </si>
+  <si>
+    <t>1.000.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bất kì thời gian nào khi khách hàng cần được tư vấn </t>
+  </si>
+  <si>
+    <t>Kênh xúc tiến</t>
+  </si>
+  <si>
+    <t>1.000.000 – 2.000.000</t>
   </si>
 </sst>
 </file>
@@ -144,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +253,35 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1C1E21"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF050505"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -229,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -289,71 +358,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -398,12 +408,47 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -427,26 +472,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -464,63 +496,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ke hoach trien khai"/>
-      <sheetName val="đầu tư ban đầu"/>
-      <sheetName val="nguồn vốn"/>
-      <sheetName val="thoi gian khấu hao"/>
-      <sheetName val="doanh thu"/>
-      <sheetName val="chi phí hoạt động"/>
-      <sheetName val="thu hồi"/>
-      <sheetName val="thuế"/>
-      <sheetName val="tra nợ vay"/>
-      <sheetName val="công thức"/>
-      <sheetName val="thu nhập"/>
-      <sheetName val="Dòng tiền"/>
-      <sheetName val="điểm hòa vốn"/>
-      <sheetName val="phân tích rủi ro"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="8">
-          <cell r="B8">
-            <v>1920000000</v>
-          </cell>
-          <cell r="C8">
-            <v>2496000000</v>
-          </cell>
-          <cell r="D8">
-            <v>3244800000</v>
-          </cell>
-          <cell r="E8">
-            <v>4218240000</v>
-          </cell>
-          <cell r="F8">
-            <v>5483712000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -789,7 +764,7 @@
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -800,20 +775,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="1">
         <f>SUM(C4:C9)</f>
         <v>107000000</v>
@@ -825,10 +800,10 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="4">
         <v>15000000</v>
       </c>
@@ -839,10 +814,10 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="4">
         <v>1500000</v>
       </c>
@@ -853,10 +828,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="4">
         <v>1000000</v>
       </c>
@@ -867,10 +842,10 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="4">
         <v>7000000</v>
       </c>
@@ -881,10 +856,10 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="4">
         <v>80000000</v>
       </c>
@@ -895,10 +870,10 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="4">
         <v>2500000</v>
       </c>
@@ -909,10 +884,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="6">
         <v>0.1</v>
       </c>
@@ -961,23 +936,18 @@
         <v>14</v>
       </c>
       <c r="B13" s="12">
-        <f>C3*12</f>
         <v>1284000000</v>
       </c>
       <c r="C13" s="13">
-        <f>B13*(1+$C$10)</f>
         <v>1412400000</v>
       </c>
       <c r="D13" s="13">
-        <f t="shared" ref="D13:F13" si="0">C13*(1+$C$10)</f>
         <v>1553640000.0000002</v>
       </c>
       <c r="E13" s="13">
-        <f t="shared" si="0"/>
         <v>1709004000.0000005</v>
       </c>
       <c r="F13" s="13">
-        <f t="shared" si="0"/>
         <v>1879904400.0000007</v>
       </c>
     </row>
@@ -986,23 +956,18 @@
         <v>15</v>
       </c>
       <c r="B14" s="12">
-        <f>C11*'[1]doanh thu'!B8</f>
         <v>384000000</v>
       </c>
       <c r="C14" s="13">
-        <f>C11*'[1]doanh thu'!C8</f>
         <v>499200000</v>
       </c>
       <c r="D14" s="13">
-        <f>C11*'[1]doanh thu'!D8</f>
         <v>648960000</v>
       </c>
       <c r="E14" s="13">
-        <f>C11*'[1]doanh thu'!E8</f>
         <v>843648000</v>
       </c>
       <c r="F14" s="13">
-        <f>C11*'[1]doanh thu'!F8</f>
         <v>1096742400</v>
       </c>
     </row>
@@ -1011,23 +976,18 @@
         <v>16</v>
       </c>
       <c r="B15" s="15">
-        <f>SUM(B13:B14)</f>
         <v>1668000000</v>
       </c>
       <c r="C15" s="15">
-        <f t="shared" ref="C15:F15" si="1">SUM(C13:C14)</f>
         <v>1911600000</v>
       </c>
       <c r="D15" s="15">
-        <f t="shared" si="1"/>
         <v>2202600000</v>
       </c>
       <c r="E15" s="15">
-        <f t="shared" si="1"/>
         <v>2552652000.0000005</v>
       </c>
       <c r="F15" s="15">
-        <f t="shared" si="1"/>
         <v>2976646800.000001</v>
       </c>
     </row>
@@ -1049,94 +1009,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA72920-98B1-47F3-8E35-46C8283B723A}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="22" customWidth="1"/>
     <col min="2" max="2" width="43.296875" customWidth="1"/>
     <col min="3" max="3" width="37.796875" customWidth="1"/>
     <col min="4" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="33.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+    <row r="3" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31" t="s">
+    <row r="4" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="32" t="s">
+    <row r="5" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="38">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="33"/>
-      <c r="C6" t="s">
+    <row r="6" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27" t="s">
+    <row r="7" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="38">
+        <v>3</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+    <row r="8" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16" t="s">
+    <row r="9" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
+        <v>4</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="19" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26">
+        <v>5</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1150,4 +1144,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4656378C-8B5C-4BF1-80FD-BAA1A55F36E8}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.8984375" customWidth="1"/>
+    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
done tuan 3 more
</commit_message>
<xml_diff>
--- a/tuan 3 add.xlsx
+++ b/tuan 3 add.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1EE11-FD70-4FF2-B7F8-38995406478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F552FC7-07C4-49D5-B4E0-33167EA3F8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
     <sheet name="2.MoTaSP" sheetId="2" r:id="rId2"/>
-    <sheet name="4.KeHoachXucTien" sheetId="3" r:id="rId3"/>
+    <sheet name="3.GiaCaSanPham" sheetId="6" r:id="rId3"/>
+    <sheet name="4.KeHoachXucTien" sheetId="3" r:id="rId4"/>
+    <sheet name="tuan3.6.KenhPPGianTiep" sheetId="5" r:id="rId5"/>
+    <sheet name="tuan3.6.KenhPPTrucTiep" sheetId="4" r:id="rId6"/>
+    <sheet name="tuan3.7.danhMucThietBi" sheetId="7" r:id="rId7"/>
+    <sheet name="6.MayMoc" sheetId="10" r:id="rId8"/>
+    <sheet name="7.LietKeNhanSu" sheetId="8" r:id="rId9"/>
+    <sheet name="8.CheDoKhenThuong" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="167">
   <si>
     <t>(5) Chi phí hoạt động</t>
   </si>
@@ -175,6 +182,387 @@
   </si>
   <si>
     <t>1.000.000 – 2.000.000</t>
+  </si>
+  <si>
+    <t>Địa chỉ đặt cửa hàng</t>
+  </si>
+  <si>
+    <t>Diện tích sàn(m2)</t>
+  </si>
+  <si>
+    <t>Tiền thuê/Tháng</t>
+  </si>
+  <si>
+    <t>Dự đoán danh thu</t>
+  </si>
+  <si>
+    <t>54 Lý Thường kiệt, tp HCM</t>
+  </si>
+  <si>
+    <t>8 000 000</t>
+  </si>
+  <si>
+    <t>2 năm</t>
+  </si>
+  <si>
+    <t>28 000 000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 lê lợi , Tp Mỹ tho </t>
+  </si>
+  <si>
+    <t>7 000 000</t>
+  </si>
+  <si>
+    <t>22 000 000</t>
+  </si>
+  <si>
+    <t>76 hùng vương, TP HCM</t>
+  </si>
+  <si>
+    <t>9 000 000</t>
+  </si>
+  <si>
+    <t>25 000 000</t>
+  </si>
+  <si>
+    <t>5 Cô Giang, TP HCM</t>
+  </si>
+  <si>
+    <t>10 000 000</t>
+  </si>
+  <si>
+    <t>35 000 000</t>
+  </si>
+  <si>
+    <t>Hệ thống kênh gián tiếp</t>
+  </si>
+  <si>
+    <t>Chi phí xây dựng kênh</t>
+  </si>
+  <si>
+    <t>Dự đoán doanh thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kênh truyền thống </t>
+  </si>
+  <si>
+    <t>1 năm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kênh hiện đại </t>
+  </si>
+  <si>
+    <t>15 000 000</t>
+  </si>
+  <si>
+    <t>27 000 000</t>
+  </si>
+  <si>
+    <t>Các kênh khác</t>
+  </si>
+  <si>
+    <t>20 000 000</t>
+  </si>
+  <si>
+    <t>Sản phẩm/ dịch vụ
+hoặc chủng loại sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá thành </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá bán </t>
+  </si>
+  <si>
+    <t>Giá đối thủ cạnh tranh 1</t>
+  </si>
+  <si>
+    <t>Giá đối thủ cạnh tranh 2</t>
+  </si>
+  <si>
+    <t>Gói STARTUP</t>
+  </si>
+  <si>
+    <t>990,000đ</t>
+  </si>
+  <si>
+    <t>Gói PRO</t>
+  </si>
+  <si>
+    <t>3,490,000đ</t>
+  </si>
+  <si>
+    <t>3,299,000đ</t>
+  </si>
+  <si>
+    <t>5,000,000đ</t>
+  </si>
+  <si>
+    <t>Gói ECOMMERCE</t>
+  </si>
+  <si>
+    <t>5,990,000đ</t>
+  </si>
+  <si>
+    <t>8,990,000đ</t>
+  </si>
+  <si>
+    <t>Gói BUSINESS</t>
+  </si>
+  <si>
+    <t>6,990,000đ</t>
+  </si>
+  <si>
+    <t>9,990,000đ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Website lẻ, mẫu sẵn </t>
+  </si>
+  <si>
+    <t>500,000đ - 3,000,000đ</t>
+  </si>
+  <si>
+    <t>500,000đ - 2,000,000đ</t>
+  </si>
+  <si>
+    <t>Các chính sách ưu đãi</t>
+  </si>
+  <si>
+    <t>Hình thức ưu đãi</t>
+  </si>
+  <si>
+    <t>Đối tượng khách hàng</t>
+  </si>
+  <si>
+    <t>Giảm giá ở các dịp lễ</t>
+  </si>
+  <si>
+    <t>5%, 10%</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>Bán chịu</t>
+  </si>
+  <si>
+    <t>Trả chậm sau 1 tháng</t>
+  </si>
+  <si>
+    <t>Hỗ trợ doanh nghiệp mùa covid</t>
+  </si>
+  <si>
+    <t>Giảm cái loại phí bảo trì</t>
+  </si>
+  <si>
+    <t>Khách hàng thân thiết</t>
+  </si>
+  <si>
+    <t>Hỗ trợ đặc biệt,
+ưu đãi mỗi 3 tháng</t>
+  </si>
+  <si>
+    <t>Máy móc, trang thiết bị, công nghệ</t>
+  </si>
+  <si>
+    <t>Tên máy móc, thiết bị</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Đơn giá VND</t>
+  </si>
+  <si>
+    <t>Thành tiền VND</t>
+  </si>
+  <si>
+    <t>Máy lạnh</t>
+  </si>
+  <si>
+    <t>Bàn ghế</t>
+  </si>
+  <si>
+    <t>Tủ lạnh</t>
+  </si>
+  <si>
+    <t>Máy in</t>
+  </si>
+  <si>
+    <t>Bảng hiệu</t>
+  </si>
+  <si>
+    <t>Máy chấm công</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Máy tính</t>
+  </si>
+  <si>
+    <t>Tủ nhân viên</t>
+  </si>
+  <si>
+    <t>Tổng Cộng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BẢNG LIỆT KÊ NHÂN SỰ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vị trí công việc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số lượng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiêu chuẩn công việc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảng mô tả công việc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giám đốc </t>
+  </si>
+  <si>
+    <t>Trình độ đại học.
+Giỏi về công nghệ.
+Biết lập trình, viết code.
+Sáng tạo, siêng năng, chịu khó, hòa đồng có kinh nghiệm am hiểu nhiều lĩnh vực.</t>
+  </si>
+  <si>
+    <t>Xác định mục tiêu và phương hướng phát triển.
+Lập kế hoạch và định hướng.
+Điều hành toàn bộ họat động và chịu trách nhiệm doanh số, lợi nhuận, hướng phát triển, tăng trưởng.
+Lập kế hoạch kinh doanh và marketing.
+Quản lý nhân viên.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhân viên tư vấn, kế toán </t>
+  </si>
+  <si>
+    <t>Là nữ Trình đô đại học.
+Siêng năng, chịu khó, trung thực, giỏi giao tiếp, hòa đồng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tư vấn chăm sóc khách hàng, tính toán thu và chi. </t>
+  </si>
+  <si>
+    <t>Nhân viên làm việc về web</t>
+  </si>
+  <si>
+    <t>Trình độ đại học.
+Giỏi về công nghệ.
+Biết lập trình viết code.
+sáng tạo, siêng năng, chịu khó, hòa đồng có kinh nghiệm.</t>
+  </si>
+  <si>
+    <t>Thiết kế sản phẩm mẫu.
+Làm việc về web về code thiết kế tất cả các trang mà các hàng yêu cầu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhân viên bảo trì web  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bảo trì web tránh những trường hợp 
+sập hoặc bị đánh cắp.</t>
+  </si>
+  <si>
+    <t>Trình độ đại học.
+Giỏi về công nghệ.
+Biết lập trình, viết code, sáng tạo siêng năng, chịu khó, hòa đồng có kinh nghiệm.</t>
+  </si>
+  <si>
+    <t>BẢNG LIỆT KÊ CHẾ ĐỘ KHEN THƯỞNG, TRỢ CẤP CÔNG VIỆC</t>
+  </si>
+  <si>
+    <t>Việc khen thưởng</t>
+  </si>
+  <si>
+    <t>Khen thưởng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm việc chuyên cần </t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/30 ngày  </t>
+  </si>
+  <si>
+    <t>500.000đ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuối tuần </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chủ nhật </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nghỉ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lễ tết  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lễ tết </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hưởng lương như ngày thường </t>
+  </si>
+  <si>
+    <t>Đầu tư thiết bị</t>
+  </si>
+  <si>
+    <t>Đơn giá</t>
+  </si>
+  <si>
+    <t>Chi phí đầu tư</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Máy tính </t>
+  </si>
+  <si>
+    <t>Máy chiếu</t>
+  </si>
+  <si>
+    <t>Máy lọc nước</t>
+  </si>
+  <si>
+    <t>Máy chủ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Máy điều hòa </t>
+  </si>
+  <si>
+    <t>Bộ phát wifi</t>
+  </si>
+  <si>
+    <t>Bàn</t>
+  </si>
+  <si>
+    <t>Ghế</t>
+  </si>
+  <si>
+    <t>Điện thoại công ty</t>
+  </si>
+  <si>
+    <t>Tủ đựng hồ sơ</t>
+  </si>
+  <si>
+    <t>Thiết bị PCCC</t>
+  </si>
+  <si>
+    <t>Hạng mục xây dựng</t>
+  </si>
+  <si>
+    <t>Mặc bằng</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Cải tạo mặt bằng và thiết kế</t>
   </si>
 </sst>
 </file>
@@ -184,7 +572,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +671,31 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times  New Roman"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF111111"/>
+      <name val="Times  New Roman"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -359,11 +772,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -450,6 +864,52 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -477,13 +937,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{20A3302F-8814-4C24-93B5-FACAC9162863}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -767,28 +1261,28 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="12.09765625" customWidth="1"/>
     <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:6" ht="16.8">
+      <c r="A2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.399999999999999">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="1">
         <f>SUM(C4:C9)</f>
         <v>107000000</v>
@@ -799,11 +1293,11 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+    <row r="4" spans="1:6" ht="17.399999999999999">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="4">
         <v>15000000</v>
       </c>
@@ -813,11 +1307,11 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:6" ht="17.399999999999999">
+      <c r="A5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="34"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="4">
         <v>1500000</v>
       </c>
@@ -827,11 +1321,11 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+    <row r="6" spans="1:6" ht="17.399999999999999">
+      <c r="A6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="4">
         <v>1000000</v>
       </c>
@@ -841,11 +1335,11 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:6" ht="17.399999999999999">
+      <c r="A7" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="4">
         <v>7000000</v>
       </c>
@@ -855,11 +1349,11 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+    <row r="8" spans="1:6" ht="17.399999999999999">
+      <c r="A8" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="4">
         <v>80000000</v>
       </c>
@@ -869,11 +1363,11 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:6" ht="17.399999999999999">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="4">
         <v>2500000</v>
       </c>
@@ -883,11 +1377,11 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+    <row r="10" spans="1:6" ht="17.399999999999999">
+      <c r="A10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="6">
         <v>0.1</v>
       </c>
@@ -897,7 +1391,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="17.399999999999999">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -911,7 +1405,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.8">
       <c r="A12" s="9" t="s">
         <v>13</v>
       </c>
@@ -931,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="33.6">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -951,7 +1445,7 @@
         <v>1879904400.0000007</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="33.6">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -971,7 +1465,7 @@
         <v>1096742400</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="50.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="50.4">
       <c r="A15" s="14" t="s">
         <v>16</v>
       </c>
@@ -1007,6 +1501,110 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30461BD0-3BC7-42C1-9964-CD25F35D452C}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.05" customHeight="1">
+      <c r="A1" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" ht="22.05" customHeight="1">
+      <c r="A2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+    </row>
+    <row r="3" spans="1:7" ht="22.05" customHeight="1">
+      <c r="A3" s="42">
+        <v>1</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:7" ht="22.05" customHeight="1">
+      <c r="A4" s="42">
+        <v>2</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+    </row>
+    <row r="5" spans="1:7" ht="22.05" customHeight="1">
+      <c r="A5" s="42">
+        <v>3</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA72920-98B1-47F3-8E35-46C8283B723A}">
   <dimension ref="A1:C13"/>
@@ -1015,7 +1613,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="7.5" style="22" customWidth="1"/>
     <col min="2" max="2" width="43.296875" customWidth="1"/>
@@ -1023,7 +1621,7 @@
     <col min="4" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="36.6" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
@@ -1034,68 +1632,68 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
+    <row r="2" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="53" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="37"/>
+    <row r="3" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A3" s="54"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="37"/>
+    <row r="4" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A4" s="54"/>
+      <c r="B4" s="53"/>
       <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+    <row r="5" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A5" s="54">
         <v>2</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="54" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
+    <row r="6" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A6" s="54"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+    <row r="7" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A7" s="54">
         <v>3</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="54" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
+    <row r="8" spans="1:3" ht="43.95" customHeight="1">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="43.95" customHeight="1">
       <c r="A9" s="26">
         <v>4</v>
       </c>
@@ -1106,7 +1704,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="43.95" customHeight="1">
       <c r="A10" s="26">
         <v>5</v>
       </c>
@@ -1117,17 +1715,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="43.95" customHeight="1">
       <c r="A11" s="21"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
     </row>
-    <row r="12" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.95" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="1:3" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="43.95" customHeight="1">
       <c r="A13" s="21"/>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1147,22 +1745,215 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B1335E-E48B-438A-9BCF-82EBC9A27991}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="26.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" customWidth="1"/>
+    <col min="5" max="5" width="19.8984375" customWidth="1"/>
+    <col min="6" max="6" width="20.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32.25" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="22">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="22">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="22">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="27.6">
+      <c r="A14" s="28">
+        <v>4</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4656378C-8B5C-4BF1-80FD-BAA1A55F36E8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="20.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69921875" customWidth="1"/>
     <col min="3" max="3" width="29.8984375" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="33.6">
       <c r="A1" s="29" t="s">
         <v>17</v>
       </c>
@@ -1176,53 +1967,890 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="33.6">
       <c r="A2" s="27">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="30" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="33.6">
       <c r="A3" s="27">
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="33.6">
       <c r="A4" s="27">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="30" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.4" customHeight="1">
       <c r="A5" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C10BAE3-57DC-4EB7-9546-93E167657BA2}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" style="31"/>
+    <col min="2" max="3" width="22.59765625" style="31" customWidth="1"/>
+    <col min="4" max="4" width="17.69921875" style="31" customWidth="1"/>
+    <col min="5" max="5" width="18.296875" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CD66FC-52B5-406F-B40F-4BD9B0893988}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="7.69921875" style="31" customWidth="1"/>
+    <col min="2" max="2" width="25" style="31" customWidth="1"/>
+    <col min="3" max="3" width="16" style="31" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="18.09765625" style="31" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" style="31" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="31">
+        <v>50</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="31">
+        <v>50</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="31">
+        <v>60</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="31">
+        <v>4</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="31">
+        <v>50</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE3BA39-1B55-4D94-A283-05E2A3B791CD}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" customHeight="1">
+      <c r="A1" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="37">
+        <v>5</v>
+      </c>
+      <c r="C3" s="39">
+        <v>8000000</v>
+      </c>
+      <c r="D3" s="40">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="37">
+        <v>10</v>
+      </c>
+      <c r="C4" s="39">
+        <v>1500000</v>
+      </c>
+      <c r="D4" s="40">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="37">
+        <v>2</v>
+      </c>
+      <c r="C5" s="39">
+        <v>10000000</v>
+      </c>
+      <c r="D5" s="40">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="37">
+        <v>3</v>
+      </c>
+      <c r="C6" s="39">
+        <v>3400000</v>
+      </c>
+      <c r="D6" s="40">
+        <v>10200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="37">
+        <v>2</v>
+      </c>
+      <c r="C7" s="39">
+        <v>1000000</v>
+      </c>
+      <c r="D7" s="40">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="37">
+        <v>1</v>
+      </c>
+      <c r="C8" s="39">
+        <v>2500000</v>
+      </c>
+      <c r="D8" s="40">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="37">
+        <v>4</v>
+      </c>
+      <c r="C9" s="39">
+        <v>3200000</v>
+      </c>
+      <c r="D9" s="40">
+        <v>12800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="37">
+        <v>10</v>
+      </c>
+      <c r="C10" s="39">
+        <v>12000000</v>
+      </c>
+      <c r="D10" s="40">
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
+      <c r="A11" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="37">
+        <v>12</v>
+      </c>
+      <c r="C11" s="39">
+        <v>500000</v>
+      </c>
+      <c r="D11" s="40">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" customHeight="1">
+      <c r="A12" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="40">
+        <v>228500000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9164778D-6E59-43BB-9718-81963B27623F}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="2" width="19.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.8">
+      <c r="A1" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.8">
+      <c r="A2" s="61">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="59">
+        <v>8</v>
+      </c>
+      <c r="D2" s="60">
+        <v>30000000</v>
+      </c>
+      <c r="E2" s="60">
+        <f>C2*D2</f>
+        <v>240000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.8">
+      <c r="A3" s="61">
+        <v>2</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="59">
+        <v>2</v>
+      </c>
+      <c r="D3" s="60">
+        <v>5000000</v>
+      </c>
+      <c r="E3" s="60">
+        <f>C3*D3</f>
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.8">
+      <c r="A4" s="61">
+        <v>3</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="59">
+        <v>1</v>
+      </c>
+      <c r="D4" s="60">
+        <v>10000000</v>
+      </c>
+      <c r="E4" s="60">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.8">
+      <c r="A5" s="61">
+        <v>4</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="59">
+        <v>1</v>
+      </c>
+      <c r="D5" s="60">
+        <v>8200000</v>
+      </c>
+      <c r="E5" s="60">
+        <v>8200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8">
+      <c r="A6" s="61">
+        <v>5</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="59">
+        <v>1</v>
+      </c>
+      <c r="D6" s="60">
+        <v>80000000</v>
+      </c>
+      <c r="E6" s="60">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.8">
+      <c r="A7" s="61">
+        <v>6</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="59">
+        <v>1</v>
+      </c>
+      <c r="D7" s="60">
+        <v>6450000</v>
+      </c>
+      <c r="E7" s="60">
+        <v>6400000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8">
+      <c r="A8" s="61">
+        <v>7</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="59">
+        <v>2</v>
+      </c>
+      <c r="D8" s="60">
+        <v>550000</v>
+      </c>
+      <c r="E8" s="60">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.8">
+      <c r="A9" s="61">
+        <v>8</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="59">
+        <v>1</v>
+      </c>
+      <c r="D9" s="60">
+        <v>300000</v>
+      </c>
+      <c r="E9" s="60">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.8">
+      <c r="A10" s="61">
+        <v>9</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="59">
+        <v>9</v>
+      </c>
+      <c r="D10" s="60">
+        <v>1500000</v>
+      </c>
+      <c r="E10" s="60">
+        <f>D10*C10</f>
+        <v>13500000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.8">
+      <c r="A11" s="61">
+        <v>10</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="59">
+        <v>9</v>
+      </c>
+      <c r="D11" s="60">
+        <v>2000000</v>
+      </c>
+      <c r="E11" s="60">
+        <f>C11*D11</f>
+        <v>18000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.8">
+      <c r="A12" s="61">
+        <v>11</v>
+      </c>
+      <c r="B12" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="59">
+        <v>1</v>
+      </c>
+      <c r="D12" s="60">
+        <v>500000</v>
+      </c>
+      <c r="E12" s="60">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.8">
+      <c r="A13" s="61">
+        <v>12</v>
+      </c>
+      <c r="B13" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="59">
+        <v>1</v>
+      </c>
+      <c r="D13" s="60">
+        <v>8000000</v>
+      </c>
+      <c r="E13" s="60">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.8">
+      <c r="A14" s="61">
+        <v>13</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="59">
+        <v>1</v>
+      </c>
+      <c r="D14" s="60">
+        <v>4000000</v>
+      </c>
+      <c r="E14" s="60">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.8">
+      <c r="A18" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.8">
+      <c r="A19" s="63">
+        <v>1</v>
+      </c>
+      <c r="B19" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="66">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.8">
+      <c r="A20" s="63">
+        <v>2</v>
+      </c>
+      <c r="B20" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="65"/>
+      <c r="D20" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="66">
+        <v>20000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA379DE-4BF8-46D1-97D2-2B2EEF4B5E52}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.59765625" customWidth="1"/>
+    <col min="3" max="3" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="43.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.8">
+      <c r="A1" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.8">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.8">
+      <c r="A3" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="117.6">
+      <c r="A4" s="42">
+        <v>1</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="50.4">
+      <c r="A5" s="42">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="42">
+        <v>1</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="84">
+      <c r="A6" s="42">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="42">
+        <v>4</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="84">
+      <c r="A7" s="42">
+        <v>4</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="42">
+        <v>1</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix (ppt): done phan 2
</commit_message>
<xml_diff>
--- a/tuan 3 add.xlsx
+++ b/tuan 3 add.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\khoi nghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F552FC7-07C4-49D5-B4E0-33167EA3F8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D140D8-0F37-433A-808F-D8CE7395BA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="168">
   <si>
     <t>(5) Chi phí hoạt động</t>
   </si>
@@ -341,12 +341,6 @@
     <t>5%, 10%</t>
   </si>
   <si>
-    <t>Khách hàng</t>
-  </si>
-  <si>
-    <t>Bán chịu</t>
-  </si>
-  <si>
     <t>Trả chậm sau 1 tháng</t>
   </si>
   <si>
@@ -357,10 +351,6 @@
   </si>
   <si>
     <t>Khách hàng thân thiết</t>
-  </si>
-  <si>
-    <t>Hỗ trợ đặc biệt,
-ưu đãi mỗi 3 tháng</t>
   </si>
   <si>
     <t>Máy móc, trang thiết bị, công nghệ</t>
@@ -563,6 +553,18 @@
   </si>
   <si>
     <t>Cải tạo mặt bằng và thiết kế</t>
+  </si>
+  <si>
+    <t>Khách hàng cũ</t>
+  </si>
+  <si>
+    <t>Bán bán trả sau</t>
+  </si>
+  <si>
+    <t>Ưu đãi hàng tháng</t>
+  </si>
+  <si>
+    <t>Hỗ trợ đặc biệt, ưu đãi mỗi 3 tháng</t>
   </si>
 </sst>
 </file>
@@ -777,7 +779,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -877,12 +879,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -910,6 +906,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -940,38 +957,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1269,20 +1265,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="16.8">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="1">
         <f>SUM(C4:C9)</f>
         <v>107000000</v>
@@ -1294,10 +1290,10 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="17.399999999999999">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="50"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="4">
         <v>15000000</v>
       </c>
@@ -1308,10 +1304,10 @@
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="17.399999999999999">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="50"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="4">
         <v>1500000</v>
       </c>
@@ -1322,10 +1318,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="17.399999999999999">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="50"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="4">
         <v>1000000</v>
       </c>
@@ -1336,10 +1332,10 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="17.399999999999999">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="50"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="4">
         <v>7000000</v>
       </c>
@@ -1350,10 +1346,10 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="17.399999999999999">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="50"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="4">
         <v>80000000</v>
       </c>
@@ -1364,10 +1360,10 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="17.399999999999999">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="4">
         <v>2500000</v>
       </c>
@@ -1378,10 +1374,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="17.399999999999999">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="6">
         <v>0.1</v>
       </c>
@@ -1518,79 +1514,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.05" customHeight="1">
-      <c r="A1" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="A1" s="64" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" ht="22.05" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="43" t="s">
-        <v>139</v>
+      <c r="D2" s="41" t="s">
+        <v>136</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="22.05" customHeight="1">
-      <c r="A3" s="42">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>142</v>
+      <c r="B3" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>139</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="22.05" customHeight="1">
-      <c r="A4" s="42">
+      <c r="A4" s="40">
         <v>2</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4" s="43" t="s">
-        <v>145</v>
+      <c r="B4" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>142</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
     </row>
     <row r="5" spans="1:7" ht="22.05" customHeight="1">
-      <c r="A5" s="42">
+      <c r="A5" s="40">
         <v>3</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>148</v>
+      <c r="B5" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>145</v>
       </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
@@ -1633,10 +1629,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A2" s="54">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="58" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -1644,24 +1640,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A4" s="54"/>
-      <c r="B4" s="53"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A5" s="54">
+      <c r="A5" s="59">
         <v>2</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="59" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -1669,17 +1665,17 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A7" s="54">
+      <c r="A7" s="59">
         <v>3</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="59" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -1687,8 +1683,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.95" customHeight="1">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="18" t="s">
         <v>29</v>
       </c>
@@ -1748,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B1335E-E48B-438A-9BCF-82EBC9A27991}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1887,7 +1883,7 @@
         <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1895,13 +1891,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1909,27 +1905,27 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
         <v>101</v>
       </c>
-      <c r="C13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="27.6">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="28">
         <v>4</v>
       </c>
-      <c r="B14" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="35" t="s">
-        <v>98</v>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2248,160 +2244,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-    </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="37" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="B3" s="35">
+        <v>5</v>
+      </c>
+      <c r="C3" s="37">
+        <v>8000000</v>
+      </c>
+      <c r="D3" s="38">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15">
+      <c r="A4" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="B4" s="35">
+        <v>10</v>
+      </c>
+      <c r="C4" s="37">
+        <v>1500000</v>
+      </c>
+      <c r="D4" s="38">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="35" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3" s="37" t="s">
+      <c r="B5" s="35">
+        <v>2</v>
+      </c>
+      <c r="C5" s="37">
+        <v>10000000</v>
+      </c>
+      <c r="D5" s="38">
+        <v>20000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15">
+      <c r="A6" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="37">
-        <v>5</v>
-      </c>
-      <c r="C3" s="39">
-        <v>8000000</v>
-      </c>
-      <c r="D3" s="40">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15">
-      <c r="A4" s="37" t="s">
+      <c r="B6" s="35">
+        <v>3</v>
+      </c>
+      <c r="C6" s="37">
+        <v>3400000</v>
+      </c>
+      <c r="D6" s="38">
+        <v>10200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15">
+      <c r="A7" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="37">
+      <c r="B7" s="35">
+        <v>2</v>
+      </c>
+      <c r="C7" s="37">
+        <v>1000000</v>
+      </c>
+      <c r="D7" s="38">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15">
+      <c r="A8" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="35">
+        <v>1</v>
+      </c>
+      <c r="C8" s="37">
+        <v>2500000</v>
+      </c>
+      <c r="D8" s="38">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15">
+      <c r="A9" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="35">
+        <v>4</v>
+      </c>
+      <c r="C9" s="37">
+        <v>3200000</v>
+      </c>
+      <c r="D9" s="38">
+        <v>12800000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15">
+      <c r="A10" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="35">
         <v>10</v>
       </c>
-      <c r="C4" s="39">
-        <v>1500000</v>
-      </c>
-      <c r="D4" s="40">
-        <v>15000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="37">
-        <v>2</v>
-      </c>
-      <c r="C5" s="39">
-        <v>10000000</v>
-      </c>
-      <c r="D5" s="40">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="37">
-        <v>3</v>
-      </c>
-      <c r="C6" s="39">
-        <v>3400000</v>
-      </c>
-      <c r="D6" s="40">
-        <v>10200000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="A7" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="37">
-        <v>2</v>
-      </c>
-      <c r="C7" s="39">
-        <v>1000000</v>
-      </c>
-      <c r="D7" s="40">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8" s="37" t="s">
+      <c r="C10" s="37">
+        <v>12000000</v>
+      </c>
+      <c r="D10" s="38">
+        <v>120000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
+      <c r="A11" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="37">
-        <v>1</v>
-      </c>
-      <c r="C8" s="39">
-        <v>2500000</v>
-      </c>
-      <c r="D8" s="40">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" s="37" t="s">
+      <c r="B11" s="35">
+        <v>12</v>
+      </c>
+      <c r="C11" s="37">
+        <v>500000</v>
+      </c>
+      <c r="D11" s="38">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" customHeight="1">
+      <c r="A12" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="37">
-        <v>4</v>
-      </c>
-      <c r="C9" s="39">
-        <v>3200000</v>
-      </c>
-      <c r="D9" s="40">
-        <v>12800000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="37">
-        <v>10</v>
-      </c>
-      <c r="C10" s="39">
-        <v>12000000</v>
-      </c>
-      <c r="D10" s="40">
-        <v>120000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
-      <c r="A11" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="37">
-        <v>12</v>
-      </c>
-      <c r="C11" s="39">
-        <v>500000</v>
-      </c>
-      <c r="D11" s="40">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.6" customHeight="1">
-      <c r="A12" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="40">
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="38">
         <v>228500000</v>
       </c>
     </row>
@@ -2419,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9164778D-6E59-43BB-9718-81963B27623F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:E20"/>
     </sheetView>
   </sheetViews>
@@ -2432,289 +2428,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.8">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.8">
+      <c r="A2" s="47">
+        <v>1</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.8">
-      <c r="A2" s="61">
-        <v>1</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="59">
+      <c r="C2" s="45">
         <v>8</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D2" s="46">
         <v>30000000</v>
       </c>
-      <c r="E2" s="60">
+      <c r="E2" s="46">
         <f>C2*D2</f>
         <v>240000000</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.8">
-      <c r="A3" s="61">
+      <c r="A3" s="47">
         <v>2</v>
       </c>
-      <c r="B3" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="59">
+      <c r="B3" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="45">
         <v>2</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="46">
         <v>5000000</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="46">
         <f>C3*D3</f>
         <v>10000000</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.8">
-      <c r="A4" s="61">
+      <c r="A4" s="47">
         <v>3</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="45">
+        <v>1</v>
+      </c>
+      <c r="D4" s="46">
+        <v>10000000</v>
+      </c>
+      <c r="E4" s="46">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.8">
+      <c r="A5" s="47">
+        <v>4</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="45">
+        <v>1</v>
+      </c>
+      <c r="D5" s="46">
+        <v>8200000</v>
+      </c>
+      <c r="E5" s="46">
+        <v>8200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.8">
+      <c r="A6" s="47">
+        <v>5</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="45">
+        <v>1</v>
+      </c>
+      <c r="D6" s="46">
+        <v>80000000</v>
+      </c>
+      <c r="E6" s="46">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.8">
+      <c r="A7" s="47">
+        <v>6</v>
+      </c>
+      <c r="B7" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C7" s="45">
         <v>1</v>
       </c>
-      <c r="D4" s="60">
-        <v>10000000</v>
-      </c>
-      <c r="E4" s="60">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.8">
-      <c r="A5" s="61">
-        <v>4</v>
-      </c>
-      <c r="B5" s="62" t="s">
+      <c r="D7" s="46">
+        <v>6450000</v>
+      </c>
+      <c r="E7" s="46">
+        <v>6400000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.8">
+      <c r="A8" s="47">
+        <v>7</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="45">
+        <v>2</v>
+      </c>
+      <c r="D8" s="46">
+        <v>550000</v>
+      </c>
+      <c r="E8" s="46">
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.8">
+      <c r="A9" s="47">
+        <v>8</v>
+      </c>
+      <c r="B9" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C9" s="45">
         <v>1</v>
       </c>
-      <c r="D5" s="60">
-        <v>8200000</v>
-      </c>
-      <c r="E5" s="60">
-        <v>8200000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.8">
-      <c r="A6" s="61">
-        <v>5</v>
-      </c>
-      <c r="B6" s="62" t="s">
+      <c r="D9" s="46">
+        <v>300000</v>
+      </c>
+      <c r="E9" s="46">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.8">
+      <c r="A10" s="47">
+        <v>9</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="59">
-        <v>1</v>
-      </c>
-      <c r="D6" s="60">
-        <v>80000000</v>
-      </c>
-      <c r="E6" s="60">
-        <v>80000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.8">
-      <c r="A7" s="61">
-        <v>6</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="C7" s="59">
-        <v>1</v>
-      </c>
-      <c r="D7" s="60">
-        <v>6450000</v>
-      </c>
-      <c r="E7" s="60">
-        <v>6400000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.8">
-      <c r="A8" s="61">
-        <v>7</v>
-      </c>
-      <c r="B8" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="59">
-        <v>2</v>
-      </c>
-      <c r="D8" s="60">
-        <v>550000</v>
-      </c>
-      <c r="E8" s="60">
-        <v>1100000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.8">
-      <c r="A9" s="61">
-        <v>8</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" s="59">
-        <v>1</v>
-      </c>
-      <c r="D9" s="60">
-        <v>300000</v>
-      </c>
-      <c r="E9" s="60">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.8">
-      <c r="A10" s="61">
+      <c r="C10" s="45">
         <v>9</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" s="59">
-        <v>9</v>
-      </c>
-      <c r="D10" s="60">
+      <c r="D10" s="46">
         <v>1500000</v>
       </c>
-      <c r="E10" s="60">
+      <c r="E10" s="46">
         <f>D10*C10</f>
         <v>13500000</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.8">
-      <c r="A11" s="61">
+      <c r="A11" s="47">
         <v>10</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="59">
+      <c r="B11" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="45">
         <v>9</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="46">
         <v>2000000</v>
       </c>
-      <c r="E11" s="60">
+      <c r="E11" s="46">
         <f>C11*D11</f>
         <v>18000000</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.8">
-      <c r="A12" s="61">
+      <c r="A12" s="47">
         <v>11</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="45">
+        <v>1</v>
+      </c>
+      <c r="D12" s="46">
+        <v>500000</v>
+      </c>
+      <c r="E12" s="46">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.8">
+      <c r="A13" s="47">
+        <v>12</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="45">
+        <v>1</v>
+      </c>
+      <c r="D13" s="46">
+        <v>8000000</v>
+      </c>
+      <c r="E13" s="46">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.8">
+      <c r="A14" s="47">
+        <v>13</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="45">
+        <v>1</v>
+      </c>
+      <c r="D14" s="46">
+        <v>4000000</v>
+      </c>
+      <c r="E14" s="46">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.8">
+      <c r="A18" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C18" s="62"/>
+      <c r="D18" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.8">
+      <c r="A19" s="49">
         <v>1</v>
       </c>
-      <c r="D12" s="60">
-        <v>500000</v>
-      </c>
-      <c r="E12" s="60">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.8">
-      <c r="A13" s="61">
-        <v>12</v>
-      </c>
-      <c r="B13" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="59">
-        <v>1</v>
-      </c>
-      <c r="D13" s="60">
-        <v>8000000</v>
-      </c>
-      <c r="E13" s="60">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.8">
-      <c r="A14" s="61">
-        <v>13</v>
-      </c>
-      <c r="B14" s="58" t="s">
+      <c r="C19" s="62"/>
+      <c r="D19" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="59">
-        <v>1</v>
-      </c>
-      <c r="D14" s="60">
-        <v>4000000</v>
-      </c>
-      <c r="E14" s="60">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.8">
-      <c r="A18" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="64" t="s">
+      <c r="E19" s="50">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.8">
+      <c r="A20" s="49">
+        <v>2</v>
+      </c>
+      <c r="B20" s="61" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.8">
-      <c r="A19" s="63">
-        <v>1</v>
-      </c>
-      <c r="B19" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="63" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" s="66">
-        <v>80000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.8">
-      <c r="A20" s="63">
-        <v>2</v>
-      </c>
-      <c r="B20" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="63" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="66">
+      <c r="C20" s="62"/>
+      <c r="D20" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="50">
         <v>20000000</v>
       </c>
     </row>
@@ -2747,104 +2743,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.8">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+    </row>
+    <row r="2" spans="1:5" ht="16.8">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.8">
+      <c r="A3" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.8">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.8">
-      <c r="A3" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="43" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="117.6">
+      <c r="A4" s="40">
+        <v>1</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>122</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="117.6">
-      <c r="A4" s="42">
-        <v>1</v>
-      </c>
-      <c r="B4" s="42" t="s">
-        <v>125</v>
       </c>
       <c r="C4" s="27">
         <v>1</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="50.4">
+      <c r="A5" s="40">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="40">
+        <v>1</v>
+      </c>
+      <c r="D5" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E5" s="43" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="50.4">
-      <c r="A5" s="42">
-        <v>2</v>
-      </c>
-      <c r="B5" s="23" t="s">
+    <row r="6" spans="1:5" ht="84">
+      <c r="A6" s="40">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C6" s="40">
+        <v>4</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="84">
+      <c r="A7" s="40">
+        <v>4</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="40">
         <v>1</v>
       </c>
-      <c r="D5" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="84">
-      <c r="A6" s="42">
-        <v>3</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="42">
-        <v>4</v>
-      </c>
-      <c r="D6" s="45" t="s">
+      <c r="D7" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="43" t="s">
         <v>132</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="84">
-      <c r="A7" s="42">
-        <v>4</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="42">
-        <v>1</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>